<commit_message>
Update Excel file for 1.1(a) with plot
</commit_message>
<xml_diff>
--- a/part2/part2_1a.xlsx
+++ b/part2/part2_1a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16180" tabRatio="500"/>
+    <workbookView xWindow="5600" yWindow="0" windowWidth="25360" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,6 +230,340 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Unloaded Latency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Working Set Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Latency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131072.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>262144.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>524288.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$2:$V$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.26505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.24997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.18559</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.29365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.47931</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.07318</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.73422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.77061</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.9705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.6301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.7366</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57.9186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63.5289</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.9573</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>98.7489</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>108.266</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>129.035</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128.876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2147177272"/>
+        <c:axId val="-2147422760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2147177272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Working</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Set Size (KiB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2147422760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2147422760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ns/access)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2147177272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -583,8 +917,8 @@
     <col min="15" max="15" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="28" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.83203125" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" customWidth="1"/>
     <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -2584,6 +2918,7 @@
   </sortState>
   <dataConsolidate/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>